<commit_message>
added additional class sets & datasets
</commit_message>
<xml_diff>
--- a/datasets/class_sets.xlsx
+++ b/datasets/class_sets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81658944-D9C6-4311-8EB5-0E50D7FE08C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FD27D7-D51C-44C1-AAD6-4E403C0130E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>city-19</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>count</t>
+  </si>
+  <si>
+    <t>idd-17</t>
   </si>
 </sst>
 </file>
@@ -430,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H23"/>
+  <dimension ref="B2:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,546 +446,666 @@
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D3" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G3" s="1" t="b">
-        <f>AND(C3:D3)</f>
         <v>1</v>
       </c>
       <c r="H3" s="1" t="b">
-        <f>AND(C3,E3)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="1" t="b">
+        <f>AND(F3:G3)</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="1" t="b">
+        <f>AND(F3,H3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D4" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G4" s="1" t="b">
-        <f t="shared" ref="G4:G21" si="0">AND(C4:D4)</f>
         <v>1</v>
       </c>
       <c r="H4" s="1" t="b">
-        <f t="shared" ref="H4:H21" si="1">AND(C4,E4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="1" t="b">
+        <f t="shared" ref="J4:J21" si="0">AND(F4:G4)</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="b">
+        <f t="shared" ref="K4:K21" si="1">AND(F4,H4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G5" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H5" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D6" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E6" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2"/>
+      <c r="E6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G6" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H6" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="E7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G7" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H7" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K7" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D8" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="E8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2"/>
+      <c r="E8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G8" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H8" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G9" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H9" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G10" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H10" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G11" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H11" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3" t="b">
-        <v>0</v>
+      <c r="D12" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="E12" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G12" s="3" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G13" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H13" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D14" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G14" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H14" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D15" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G15" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H15" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K15" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D16" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G16" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H16" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K16" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C17" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2"/>
+      <c r="D17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="G17" s="3" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="D18" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="F18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="3" t="b">
-        <v>0</v>
+      <c r="D19" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="E19" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="G19" s="3" t="b">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D20" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E20" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G20" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H20" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K20" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="D21" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="G21" s="1" t="b">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H21" s="1" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="1" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K21" s="1" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>25</v>
       </c>
-      <c r="B23">
+      <c r="D23">
         <v>19</v>
       </c>
-      <c r="C23">
+      <c r="E23">
+        <v>17</v>
+      </c>
+      <c r="F23">
         <v>16</v>
       </c>
-      <c r="D23">
+      <c r="G23">
         <v>16</v>
       </c>
-      <c r="E23">
+      <c r="H23">
         <v>13</v>
       </c>
-      <c r="G23">
+      <c r="J23">
         <v>15</v>
       </c>
-      <c r="H23">
+      <c r="K23">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:E21">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="D3:H21">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
test now reports results on all class subsets
</commit_message>
<xml_diff>
--- a/datasets/class_sets.xlsx
+++ b/datasets/class_sets.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FD27D7-D51C-44C1-AAD6-4E403C0130E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82903E8-26A4-4249-8784-34C32B66FA4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>city-19</t>
   </si>
@@ -433,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:K23"/>
+  <dimension ref="B2:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,19 +1103,637 @@
         <v>12</v>
       </c>
     </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>2</v>
+      </c>
+      <c r="F28" s="1">
+        <v>2</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="1">
+        <v>2</v>
+      </c>
+      <c r="K28" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
+      <c r="E29" s="1">
+        <v>3</v>
+      </c>
+      <c r="F29" s="1">
+        <v>3</v>
+      </c>
+      <c r="G29" s="1">
+        <v>3</v>
+      </c>
+      <c r="H29" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="1">
+        <v>3</v>
+      </c>
+      <c r="K29" s="3" t="b">
+        <f t="shared" ref="K27:K44" si="2">AND(F29,H29)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1">
+        <v>4</v>
+      </c>
+      <c r="E30" s="1">
+        <v>4</v>
+      </c>
+      <c r="F30" s="1">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="1">
+        <v>4</v>
+      </c>
+      <c r="K30" s="3" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1">
+        <v>5</v>
+      </c>
+      <c r="E31" s="1">
+        <v>5</v>
+      </c>
+      <c r="F31" s="1">
+        <v>5</v>
+      </c>
+      <c r="G31" s="1">
+        <v>5</v>
+      </c>
+      <c r="H31" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2"/>
+      <c r="J31" s="1">
+        <v>5</v>
+      </c>
+      <c r="K31" s="3" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="1">
+        <v>6</v>
+      </c>
+      <c r="E32" s="1">
+        <v>6</v>
+      </c>
+      <c r="F32" s="1">
+        <v>6</v>
+      </c>
+      <c r="G32" s="1">
+        <v>6</v>
+      </c>
+      <c r="H32" s="1">
+        <v>3</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="1">
+        <v>6</v>
+      </c>
+      <c r="K32" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="1">
+        <v>7</v>
+      </c>
+      <c r="E33" s="1">
+        <v>7</v>
+      </c>
+      <c r="F33" s="1">
+        <v>7</v>
+      </c>
+      <c r="G33" s="1">
+        <v>7</v>
+      </c>
+      <c r="H33" s="1">
+        <v>4</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="J33" s="1">
+        <v>7</v>
+      </c>
+      <c r="K33" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="1">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1">
+        <v>8</v>
+      </c>
+      <c r="F34" s="1">
+        <v>8</v>
+      </c>
+      <c r="G34" s="1">
+        <v>8</v>
+      </c>
+      <c r="H34" s="1">
+        <v>5</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="1">
+        <v>8</v>
+      </c>
+      <c r="K34" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="1">
+        <v>9</v>
+      </c>
+      <c r="E35" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>9</v>
+      </c>
+      <c r="G35" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="3" t="b">
+        <f t="shared" ref="J27:J44" si="3">AND(F35:G35)</f>
+        <v>0</v>
+      </c>
+      <c r="K35" s="3" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="1">
+        <v>10</v>
+      </c>
+      <c r="E36" s="1">
+        <v>9</v>
+      </c>
+      <c r="F36" s="1">
+        <v>10</v>
+      </c>
+      <c r="G36" s="1">
+        <v>9</v>
+      </c>
+      <c r="H36" s="1">
+        <v>6</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="1">
+        <v>9</v>
+      </c>
+      <c r="K36" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="1">
+        <v>11</v>
+      </c>
+      <c r="E37" s="1">
+        <v>10</v>
+      </c>
+      <c r="F37" s="1">
+        <v>11</v>
+      </c>
+      <c r="G37" s="1">
+        <v>10</v>
+      </c>
+      <c r="H37" s="1">
+        <v>7</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="1">
+        <v>10</v>
+      </c>
+      <c r="K37" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1">
+        <v>12</v>
+      </c>
+      <c r="E38" s="1">
+        <v>11</v>
+      </c>
+      <c r="F38" s="1">
+        <v>12</v>
+      </c>
+      <c r="G38" s="1">
+        <v>11</v>
+      </c>
+      <c r="H38" s="1">
+        <v>8</v>
+      </c>
+      <c r="I38" s="2"/>
+      <c r="J38" s="1">
+        <v>11</v>
+      </c>
+      <c r="K38" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="1">
+        <v>13</v>
+      </c>
+      <c r="E39" s="1">
+        <v>12</v>
+      </c>
+      <c r="F39" s="1">
+        <v>13</v>
+      </c>
+      <c r="G39" s="1">
+        <v>12</v>
+      </c>
+      <c r="H39" s="1">
+        <v>9</v>
+      </c>
+      <c r="I39" s="2"/>
+      <c r="J39" s="1">
+        <v>12</v>
+      </c>
+      <c r="K39" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="C40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" s="1">
+        <v>14</v>
+      </c>
+      <c r="E40" s="1">
+        <v>13</v>
+      </c>
+      <c r="F40" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I40" s="2"/>
+      <c r="J40" s="3" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="3" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>15</v>
+      </c>
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="1">
+        <v>15</v>
+      </c>
+      <c r="E41" s="1">
+        <v>14</v>
+      </c>
+      <c r="F41" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>13</v>
+      </c>
+      <c r="H41" s="1">
+        <v>10</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="3" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K41" s="3" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>16</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="1">
+        <v>16</v>
+      </c>
+      <c r="E42" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" s="2"/>
+      <c r="J42" s="3" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="3" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" s="1">
+        <v>17</v>
+      </c>
+      <c r="E43" s="1">
+        <v>15</v>
+      </c>
+      <c r="F43" s="1">
+        <v>14</v>
+      </c>
+      <c r="G43" s="1">
+        <v>14</v>
+      </c>
+      <c r="H43" s="1">
+        <v>11</v>
+      </c>
+      <c r="I43" s="2"/>
+      <c r="J43" s="1">
+        <v>13</v>
+      </c>
+      <c r="K43" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="1">
+        <v>18</v>
+      </c>
+      <c r="E44" s="1">
+        <v>16</v>
+      </c>
+      <c r="F44" s="1">
+        <v>15</v>
+      </c>
+      <c r="G44" s="1">
+        <v>15</v>
+      </c>
+      <c r="H44" s="1">
+        <v>12</v>
+      </c>
+      <c r="I44" s="2"/>
+      <c r="J44" s="1">
+        <v>14</v>
+      </c>
+      <c r="K44" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46">
+        <v>19</v>
+      </c>
+      <c r="E46">
+        <v>17</v>
+      </c>
+      <c r="F46">
+        <v>16</v>
+      </c>
+      <c r="G46">
+        <v>16</v>
+      </c>
+      <c r="H46">
+        <v>13</v>
+      </c>
+      <c r="J46">
+        <v>15</v>
+      </c>
+      <c r="K46">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:H21">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>